<commit_message>
Added benchmark timing doc
</commit_message>
<xml_diff>
--- a/doc/Benchmarks.xlsx
+++ b/doc/Benchmarks.xlsx
@@ -2,14 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Documents\Techy Stuff\My Programs\Haskell\MyLibraries\MapWith\NotGit\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15630" windowHeight="6840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>24be88a</t>
   </si>
@@ -162,6 +157,33 @@
   </si>
   <si>
     <t>prevNextMapWith</t>
+  </si>
+  <si>
+    <t>plus right fusion</t>
+  </si>
+  <si>
+    <t>time/s</t>
+  </si>
+  <si>
+    <t>alloc/bytes</t>
+  </si>
+  <si>
+    <t>42333cd</t>
+  </si>
+  <si>
+    <t>Based on perf\Benchmarks.hs</t>
+  </si>
+  <si>
+    <t>All run per cabal:</t>
+  </si>
+  <si>
+    <t>cabal bench benchmarks --ghc-options="-O2 -fno-prof-auto" --benchmark-options="+RTS -P"</t>
+  </si>
+  <si>
+    <t>All run twice in close succession; 2nd reading taken.</t>
+  </si>
+  <si>
+    <t>(list of 1,000,000 Ints)</t>
   </si>
 </sst>
 </file>
@@ -185,7 +207,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -203,8 +225,48 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
-      <right style="thin">
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
@@ -213,11 +275,116 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
       <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -226,63 +393,107 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -563,472 +774,566 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:O28"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="9" width="17.7109375" customWidth="1"/>
     <col min="10" max="10" width="18.140625" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E2" s="19" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="9"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="20"/>
-      <c r="G2" s="19" t="s">
+      <c r="F5" s="26"/>
+      <c r="G5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="20"/>
-      <c r="I2" t="s">
+      <c r="H5" s="26"/>
+      <c r="I5" s="11" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E3" s="2" t="s">
+      <c r="J5" s="26"/>
+    </row>
+    <row r="6" spans="1:11" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="13"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F6" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G6" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H6" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I6" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J6" s="42" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F4" s="9"/>
-      <c r="H4" s="9"/>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="D7" s="16"/>
+      <c r="E7" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F7" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G7" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="25" t="s">
+      <c r="H7" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J7" s="15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E6">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="35"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="4">
         <v>0.05</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F8" s="16">
         <v>0.06</v>
       </c>
-      <c r="G6">
+      <c r="G8" s="4">
         <v>0.06</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H8" s="16">
         <v>0.05</v>
       </c>
-      <c r="I6">
+      <c r="I8" s="4">
         <v>0.05</v>
       </c>
-      <c r="J6">
+      <c r="J8" s="49">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E7" s="1">
+      <c r="K8" s="50" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="35"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="32">
         <v>168045928</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F9" s="33">
         <v>184046160</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G9" s="32">
         <v>176045936</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H9" s="33">
         <v>184046128</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I9" s="32">
         <v>176046056</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J9" s="51">
         <v>200046112</v>
       </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C8" s="27" t="s">
+      <c r="K9" s="50" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="35"/>
+      <c r="C10" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="4" t="s">
+      <c r="D10" s="16"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E9" s="1"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="3">
+      <c r="J10" s="16"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="35"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="19">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E10" s="1"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="1">
+      <c r="J11" s="16"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="35"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="32">
         <v>168046048</v>
       </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
+      <c r="J12" s="31"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="35"/>
+      <c r="C13" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="D13" s="16"/>
+      <c r="E13" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F13" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G13" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="H13" s="15" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E12" s="3">
+      <c r="I13" s="4"/>
+      <c r="J13" s="16"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="35"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="19">
         <v>0.03</v>
       </c>
-      <c r="F12" s="13">
+      <c r="F14" s="28">
         <v>0.03</v>
       </c>
-      <c r="G12">
+      <c r="G14" s="4">
         <v>0.27</v>
       </c>
-      <c r="H12" s="9">
+      <c r="H14" s="16">
         <v>0.27</v>
       </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="8">
+      <c r="I14" s="4"/>
+      <c r="J14" s="16"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="35"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="32">
         <v>96045928</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F15" s="33">
         <v>96046168</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G15" s="32">
         <v>336045848</v>
       </c>
-      <c r="H13" s="11">
+      <c r="H15" s="33">
         <v>352046072</v>
       </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="7"/>
-      <c r="C14" s="7" t="s">
+      <c r="I15" s="30"/>
+      <c r="J15" s="31"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="35"/>
+      <c r="C16" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="15" t="s">
+      <c r="D16" s="16"/>
+      <c r="E16" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F16" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="G14" s="21" t="s">
+      <c r="G16" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H14" s="10" t="s">
+      <c r="H16" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="I16" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="J16" s="15" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="16">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="35"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="7">
         <v>0.02</v>
       </c>
-      <c r="F15" s="13">
+      <c r="F17" s="28">
         <v>0.06</v>
       </c>
-      <c r="G15" s="7">
+      <c r="G17" s="4">
         <v>0.05</v>
       </c>
-      <c r="H15" s="9">
+      <c r="H17" s="16">
         <v>0.06</v>
       </c>
-      <c r="I15">
+      <c r="I17" s="4">
         <v>0.05</v>
       </c>
-      <c r="J15">
+      <c r="J17" s="16">
         <v>0.12</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="8">
+    <row r="18" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="36"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="3">
         <v>80045928</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F18" s="25">
         <v>184046096</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G18" s="3">
         <v>136045912</v>
       </c>
-      <c r="H16" s="11">
+      <c r="H18" s="25">
         <v>144046136</v>
       </c>
-      <c r="I16" s="1">
+      <c r="I18" s="3">
         <v>136046056</v>
       </c>
-      <c r="J16" s="1">
+      <c r="J18" s="25">
         <v>384046064</v>
       </c>
     </row>
-    <row r="17" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
-    </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="D19" s="44"/>
+      <c r="E19" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F19" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G19" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="H18" s="10" t="s">
+      <c r="H19" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="I18" s="21" t="s">
+      <c r="I19" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="J18" s="21" t="s">
+      <c r="J19" s="48" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E19" s="2"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="10"/>
-    </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="35"/>
+      <c r="C20" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="14">
         <v>0.28999999999999998</v>
       </c>
-      <c r="F20" s="10">
+      <c r="F20" s="15">
         <v>0.42</v>
       </c>
       <c r="G20" s="22">
         <v>0.3</v>
       </c>
-      <c r="H20" s="10">
+      <c r="H20" s="15">
         <v>0.36</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="4">
         <v>0.81</v>
       </c>
-      <c r="J20">
+      <c r="J20" s="16">
         <v>0.75</v>
       </c>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E21" s="4">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B21" s="35"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="38">
         <v>664046080</v>
       </c>
-      <c r="F21" s="12">
+      <c r="F21" s="39">
         <v>680046320</v>
       </c>
-      <c r="G21" s="4">
+      <c r="G21" s="38">
         <v>664046120</v>
       </c>
-      <c r="H21" s="12">
+      <c r="H21" s="39">
         <v>680046320</v>
       </c>
-      <c r="I21" s="1">
+      <c r="I21" s="32">
         <v>1288046504</v>
       </c>
-      <c r="J21" s="1">
+      <c r="J21" s="33">
         <v>1320046504</v>
       </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B22" s="35"/>
+      <c r="C22" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="E22" s="23">
+      <c r="E22" s="7">
         <v>0.04</v>
       </c>
-      <c r="F22" s="24">
+      <c r="F22" s="29">
         <v>0.04</v>
       </c>
-      <c r="G22" s="23">
+      <c r="G22" s="7">
         <v>0.05</v>
       </c>
-      <c r="H22" s="24">
+      <c r="H22" s="29">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="4">
         <v>0.21</v>
       </c>
-      <c r="J22">
+      <c r="J22" s="16">
         <v>0.23</v>
       </c>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D23" s="27" t="s">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B23" s="35"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E23" s="38">
         <v>136045808</v>
       </c>
-      <c r="F23" s="12">
+      <c r="F23" s="39">
         <v>136046048</v>
       </c>
-      <c r="G23" s="4">
+      <c r="G23" s="38">
         <v>152045952</v>
       </c>
-      <c r="H23" s="12">
+      <c r="H23" s="39">
         <v>184046152</v>
       </c>
-      <c r="I23" s="1">
+      <c r="I23" s="32">
         <v>504046128</v>
       </c>
-      <c r="J23" s="1">
+      <c r="J23" s="33">
         <v>512046184</v>
       </c>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B24" s="35"/>
+      <c r="C24" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="E24" s="17">
+      <c r="E24" s="23">
         <v>0</v>
       </c>
-      <c r="F24" s="18">
+      <c r="F24" s="24">
         <v>0</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="4">
         <v>0.06</v>
       </c>
-      <c r="H24" s="9">
+      <c r="H24" s="16">
         <v>0.06</v>
       </c>
-      <c r="I24" s="17">
+      <c r="I24" s="23">
         <v>0.2</v>
       </c>
-      <c r="J24" s="17">
+      <c r="J24" s="24">
         <v>0.21</v>
       </c>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E25" s="1">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B25" s="35"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="32">
         <v>45912</v>
       </c>
-      <c r="F25" s="11">
+      <c r="F25" s="33">
         <v>46168</v>
       </c>
-      <c r="G25" s="1">
+      <c r="G25" s="32">
         <v>152045952</v>
       </c>
-      <c r="H25" s="11">
+      <c r="H25" s="33">
         <v>184046152</v>
       </c>
-      <c r="I25" s="1">
+      <c r="I25" s="32">
         <v>504046128</v>
       </c>
-      <c r="J25" s="1">
+      <c r="J25" s="33">
         <v>512046184</v>
       </c>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="F26" s="9"/>
-      <c r="H26" s="9"/>
-    </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="F27" s="9"/>
-      <c r="H27" s="9"/>
-    </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="F28" s="9"/>
-      <c r="H28" s="9"/>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B26" s="35"/>
+      <c r="C26" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E26" s="23">
+        <v>0</v>
+      </c>
+      <c r="F26" s="24">
+        <v>0</v>
+      </c>
+      <c r="G26" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H26" s="16">
+        <v>0.11</v>
+      </c>
+      <c r="I26" s="4">
+        <v>0.08</v>
+      </c>
+      <c r="J26" s="16">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="36"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="3">
+        <v>45912</v>
+      </c>
+      <c r="F27" s="25">
+        <v>46168</v>
+      </c>
+      <c r="G27" s="3">
+        <v>72045912</v>
+      </c>
+      <c r="H27" s="25">
+        <v>104046112</v>
+      </c>
+      <c r="I27" s="3">
+        <v>72046064</v>
+      </c>
+      <c r="J27" s="25">
+        <v>120046032</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F28" s="10"/>
+      <c r="H28" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>